<commit_message>
Adding starting vaccination module
</commit_message>
<xml_diff>
--- a/coefficients.xlsx
+++ b/coefficients.xlsx
@@ -134,28 +134,28 @@
         <v>2000.0</v>
       </c>
       <c r="B2" t="n">
-        <v>45.0</v>
+        <v>44.0</v>
       </c>
       <c r="C2" t="n">
-        <v>91.0</v>
+        <v>96.0</v>
       </c>
       <c r="D2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="E2" t="n">
         <v>20.0</v>
       </c>
-      <c r="E2" t="n">
-        <v>400.0</v>
-      </c>
       <c r="F2" t="n">
-        <v>0.0014132800633299136</v>
+        <v>0.006619216621862723</v>
       </c>
       <c r="G2" t="n">
-        <v>0.006393673208450246</v>
+        <v>0.09067422947244705</v>
       </c>
       <c r="H2" t="n">
-        <v>0.01020070143744024</v>
+        <v>0.09705053943736999</v>
       </c>
       <c r="I2" t="n">
-        <v>0.014823315854119312</v>
+        <v>0.03317966590840471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add smth new experiments and additional class for presentation
</commit_message>
<xml_diff>
--- a/coefficients.xlsx
+++ b/coefficients.xlsx
@@ -134,10 +134,10 @@
         <v>2000.0</v>
       </c>
       <c r="B2" t="n">
-        <v>44.0</v>
+        <v>20.0</v>
       </c>
       <c r="C2" t="n">
-        <v>96.0</v>
+        <v>74.0</v>
       </c>
       <c r="D2" t="n">
         <v>2.0</v>
@@ -146,16 +146,16 @@
         <v>20.0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.006619216621862723</v>
+        <v>0.03857059124412755</v>
       </c>
       <c r="G2" t="n">
-        <v>0.09067422947244705</v>
+        <v>0.027246838052063738</v>
       </c>
       <c r="H2" t="n">
-        <v>0.09705053943736999</v>
+        <v>0.0473148015517764</v>
       </c>
       <c r="I2" t="n">
-        <v>0.03317966590840471</v>
+        <v>0.06698136254656667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>